<commit_message>
Preprocesamiento de datos y análisis de DB_Entrenamientos
</commit_message>
<xml_diff>
--- a/data/ref/DB_Jugadores.xlsx
+++ b/data/ref/DB_Jugadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Desktop\DATA SCIENCE\PP- VOLUNTAREADO\chivas-ml\data\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F797A91-4A89-4D91-97DA-ADB57FDD5035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9991C1F7-9B69-4220-BD3E-71B4484EF1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C20D2E0F-2BDA-4007-BEF2-D22DFDF9AF6A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="103">
   <si>
     <t>ID_Jugador</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Defensor</t>
   </si>
   <si>
-    <t>Defensa</t>
-  </si>
-  <si>
     <t>https://storage.chivasdecorazon.com.mx/2018/jugadores/detalle/175.png</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t>Mediocampista</t>
   </si>
   <si>
-    <t>Medio</t>
-  </si>
-  <si>
     <t>https://storage.chivasdecorazon.com.mx/2018/jugadores/detalle/237.png</t>
   </si>
   <si>
@@ -336,6 +330,21 @@
   </si>
   <si>
     <t>Gael García</t>
+  </si>
+  <si>
+    <t>Defensa Central</t>
+  </si>
+  <si>
+    <t>Defensa Lateral</t>
+  </si>
+  <si>
+    <t>Extremo</t>
+  </si>
+  <si>
+    <t>Medio Defensivo</t>
+  </si>
+  <si>
+    <t>Medio Ofensivo</t>
   </si>
 </sst>
 </file>
@@ -731,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16BC79C7-F1E6-4D5B-8241-372AF8B999B4}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C24" zoomScale="117" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="117" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,22 +767,22 @@
         <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -802,7 +811,7 @@
         <v>7</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -831,7 +840,7 @@
         <v>9</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -857,10 +866,10 @@
         <v>6</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -883,13 +892,13 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -897,7 +906,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3">
         <v>26</v>
@@ -912,13 +921,13 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -926,7 +935,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3">
         <v>22</v>
@@ -941,13 +950,13 @@
         <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -955,7 +964,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3">
         <v>22</v>
@@ -970,13 +979,13 @@
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -984,7 +993,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3">
         <v>25</v>
@@ -999,13 +1008,13 @@
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1013,7 +1022,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3">
         <v>23</v>
@@ -1028,13 +1037,13 @@
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1042,7 +1051,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3">
         <v>23</v>
@@ -1057,13 +1066,13 @@
         <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1071,7 +1080,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3">
         <v>22</v>
@@ -1086,13 +1095,13 @@
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1100,7 +1109,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3">
         <v>24</v>
@@ -1115,13 +1124,13 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1129,7 +1138,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3">
         <v>22</v>
@@ -1144,13 +1153,13 @@
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1158,7 +1167,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="3">
         <v>29</v>
@@ -1170,16 +1179,16 @@
         <v>176</v>
       </c>
       <c r="F15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G15" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="I15" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1187,7 +1196,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3">
         <v>23</v>
@@ -1199,16 +1208,16 @@
         <v>175</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1216,7 +1225,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" s="3">
         <v>34</v>
@@ -1228,16 +1237,16 @@
         <v>171</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G17" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1245,7 +1254,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3">
         <v>30</v>
@@ -1257,16 +1266,16 @@
         <v>181</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1274,7 +1283,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C19" s="3">
         <v>30</v>
@@ -1286,16 +1295,16 @@
         <v>182</v>
       </c>
       <c r="F19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1303,7 +1312,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" s="3">
         <v>26</v>
@@ -1312,16 +1321,16 @@
         <v>176</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G20" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1329,7 +1338,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" s="3">
         <v>31</v>
@@ -1341,16 +1350,16 @@
         <v>175</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1358,7 +1367,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22" s="3">
         <v>24</v>
@@ -1370,16 +1379,16 @@
         <v>172</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G22" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1387,7 +1396,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C23" s="3">
         <v>21</v>
@@ -1399,16 +1408,16 @@
         <v>182</v>
       </c>
       <c r="F23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" t="s">
+        <v>100</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G23" t="s">
-        <v>48</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="I23" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1416,7 +1425,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C24" s="3">
         <v>34</v>
@@ -1428,16 +1437,16 @@
         <v>177</v>
       </c>
       <c r="F24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1445,7 +1454,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C25" s="3">
         <v>37</v>
@@ -1457,16 +1466,16 @@
         <v>175</v>
       </c>
       <c r="F25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1474,7 +1483,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C26" s="3">
         <v>26</v>
@@ -1486,16 +1495,16 @@
         <v>176</v>
       </c>
       <c r="F26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G26" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1503,7 +1512,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C27" s="3">
         <v>18</v>
@@ -1515,16 +1524,16 @@
         <v>167</v>
       </c>
       <c r="F27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G27" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1532,7 +1541,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C28" s="3">
         <v>23</v>
@@ -1544,16 +1553,16 @@
         <v>191</v>
       </c>
       <c r="F28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1561,7 +1570,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C29" s="3">
         <v>19</v>
@@ -1573,16 +1582,16 @@
         <v>172</v>
       </c>
       <c r="F29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G29" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1590,7 +1599,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C30" s="3">
         <v>22</v>
@@ -1602,16 +1611,16 @@
         <v>179</v>
       </c>
       <c r="F30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1619,7 +1628,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C31" s="3">
         <v>23</v>
@@ -1631,13 +1640,13 @@
         <v>173</v>
       </c>
       <c r="F31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Proceso de Análisis de DB_Entrenamientos y DB_Partidos
</commit_message>
<xml_diff>
--- a/data/ref/DB_Jugadores.xlsx
+++ b/data/ref/DB_Jugadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Desktop\DATA SCIENCE\PP- VOLUNTAREADO\chivas-ml\data\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9991C1F7-9B69-4220-BD3E-71B4484EF1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8EFCC5-AFE4-4D0D-A73F-F0F9FF5852B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C20D2E0F-2BDA-4007-BEF2-D22DFDF9AF6A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="105">
   <si>
     <t>ID_Jugador</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>Medio Ofensivo</t>
+  </si>
+  <si>
+    <t>Santiago Sandoval</t>
+  </si>
+  <si>
+    <t>https://cdn.resfu.com/img_data/players/medium/3348548.jpg?size=120x&amp;lossy=1</t>
   </si>
 </sst>
 </file>
@@ -738,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16BC79C7-F1E6-4D5B-8241-372AF8B999B4}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="117" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="117" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,6 +1653,35 @@
       </c>
       <c r="H31" s="1" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="3">
+        <v>18</v>
+      </c>
+      <c r="D32" s="2">
+        <v>56</v>
+      </c>
+      <c r="E32" s="3">
+        <v>165</v>
+      </c>
+      <c r="F32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" t="s">
+        <v>102</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I32" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1710,6 +1745,7 @@
     <hyperlink ref="I29" r:id="rId57" xr:uid="{5EC6D469-0CF4-4EA9-8CB8-FEC807E882F3}"/>
     <hyperlink ref="I30" r:id="rId58" xr:uid="{3AA3EA05-D75C-4A41-8891-EB1FAD03198C}"/>
     <hyperlink ref="H31" r:id="rId59" xr:uid="{54F4C950-18F1-4434-AD10-1107044BE9A7}"/>
+    <hyperlink ref="H32" r:id="rId60" xr:uid="{28D345E2-67CC-4128-A1D8-42D81766B9AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>